<commit_message>
New subversion.  Added versions to all windows.  Made some features of the Tardis Admin only.  Rearranged Tardis menus.  Changed the way the Start of Day launcher works.  Noticed it was skipping seconds, so I made something a little more broad scope for time.
</commit_message>
<xml_diff>
--- a/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
+++ b/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
   <si>
-    <t>Summary report for 11/10/2019 through 11/23/2019</t>
+    <t>Summary report for 11/17/2019 through 11/30/2019</t>
   </si>
   <si>
     <t>payroll_id</t>
@@ -55,10 +55,10 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>11/10/2019</t>
-  </si>
-  <si>
-    <t>11/23/2019</t>
+    <t>11/17/2019</t>
+  </si>
+  <si>
+    <t>11/30/2019</t>
   </si>
   <si>
     <t>Adam</t>
@@ -605,7 +605,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3">
-        <v>40.7</v>
+        <v>38.18</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -628,7 +628,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3">
-        <v>91</v>
+        <v>64.02</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -651,7 +651,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>17.63</v>
+        <v>33.92</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -674,7 +674,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="3">
-        <v>17.95</v>
+        <v>18.02</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -743,7 +743,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="3">
-        <v>23.77</v>
+        <v>8.970000000000001</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -789,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3">
-        <v>14.87</v>
+        <v>28.03</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -812,7 +812,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="3">
-        <v>76.2</v>
+        <v>52.18</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -881,7 +881,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="3">
-        <v>17.93</v>
+        <v>2.48</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -950,7 +950,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Made some corrections to the EOD system and how it gets triggered.  Hopefully this will make for better clock-outs
</commit_message>
<xml_diff>
--- a/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
+++ b/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamb\OneDrive\Documents\Scripts\Python\Utilities\time_lord\buildingblocks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{D16D9001-C158-4659-91B1-971FD758F879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-33090" yWindow="3495" windowWidth="28095" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
   <si>
     <t>Summary report for 11/17/2019 through 11/30/2019</t>
   </si>
@@ -125,12 +131,6 @@
   </si>
   <si>
     <t>Cummins</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Keller</t>
   </si>
   <si>
     <t>Panida</t>
@@ -211,8 +211,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +272,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -318,7 +326,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,9 +358,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,6 +410,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -559,22 +603,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -600,7 +644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -623,12 +667,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3">
-        <v>64.02</v>
+        <v>88.02</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -646,12 +690,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>33.92</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -669,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -692,7 +736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -715,7 +759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -738,12 +782,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3">
-        <v>8.970000000000001</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -761,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -784,7 +828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -807,7 +851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -830,7 +874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -853,12 +897,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>2.48</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -867,7 +911,7 @@
         <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s">
         <v>13</v>
@@ -876,21 +920,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3">
-        <v>2.48</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s">
         <v>13</v>
@@ -899,7 +943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -922,12 +966,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="D19" t="s">
         <v>44</v>
@@ -945,12 +989,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="3">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -968,7 +1012,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -991,7 +1035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1058,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>17</v>
       </c>
@@ -1025,7 +1069,7 @@
         <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
@@ -1037,7 +1081,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -1045,13 +1089,13 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s">
         <v>13</v>
@@ -1060,62 +1104,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="3" t="s">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F25" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1" t="s">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rolling out 0.3.4 before doing some heavy lifting.
</commit_message>
<xml_diff>
--- a/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
+++ b/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamb\OneDrive\Documents\Scripts\Python\Utilities\time_lord\buildingblocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{D16D9001-C158-4659-91B1-971FD758F879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{E27710B8-90CF-4664-8A9E-91BC2A37C235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33090" yWindow="3495" windowWidth="28095" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,7 +672,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3">
-        <v>88.02</v>
+        <v>80.02</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Made improvements to the EOD tool and how it responds.  Made improvements to the Tardis.  Made improvements to how things are launched and triggered by Session Lock and Unlock activity.  This is version 0.4.0
</commit_message>
<xml_diff>
--- a/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
+++ b/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamb\OneDrive\Documents\Scripts\Python\Utilities\time_lord\buildingblocks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{E27710B8-90CF-4664-8A9E-91BC2A37C235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33090" yWindow="3495" windowWidth="28095" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
   <si>
-    <t>Summary report for 11/17/2019 through 11/30/2019</t>
+    <t>Summary report for 12/1/2019 through 12/14/2019</t>
   </si>
   <si>
     <t>payroll_id</t>
@@ -61,10 +55,10 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>11/17/2019</t>
-  </si>
-  <si>
-    <t>11/30/2019</t>
+    <t>12/1/2019</t>
+  </si>
+  <si>
+    <t>12/14/2019</t>
   </si>
   <si>
     <t>Adam</t>
@@ -211,8 +205,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,14 +266,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -326,7 +312,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,27 +344,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,24 +378,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -603,22 +553,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -644,12 +594,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3">
-        <v>38.18</v>
+        <v>28.75</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -667,12 +617,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3">
-        <v>80.02</v>
+        <v>77.34999999999999</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -690,12 +640,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>33.799999999999997</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -713,12 +663,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3">
-        <v>18.02</v>
+        <v>90.88</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -736,7 +686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -759,12 +709,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>193.17</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -782,12 +732,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3">
-        <v>8.9700000000000006</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -805,7 +755,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -828,12 +778,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3">
-        <v>28.03</v>
+        <v>70.98</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -851,12 +801,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="3">
-        <v>52.18</v>
+        <v>121.77</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -874,12 +824,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>262.87</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
@@ -897,12 +847,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="3">
-        <v>2.48</v>
+        <v>147.6</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -920,7 +870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -943,12 +893,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>108.53</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -966,12 +916,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="3">
-        <v>0.33</v>
+        <v>108.32</v>
       </c>
       <c r="D19" t="s">
         <v>44</v>
@@ -989,12 +939,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>177.88</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -1012,12 +962,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="3">
-        <v>0</v>
+        <v>218.3</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
@@ -1035,12 +985,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="B22" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>273.52</v>
       </c>
       <c r="D22" t="s">
         <v>50</v>
@@ -1058,12 +1008,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="3">
-        <v>0</v>
+        <v>174.52</v>
       </c>
       <c r="D23" t="s">
         <v>52</v>
@@ -1081,7 +1031,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -1104,37 +1054,37 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
0.4.1 important update.  The ability to have people restart their Tardis without restarting their computer.
</commit_message>
<xml_diff>
--- a/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
+++ b/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
@@ -645,7 +645,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>107</v>
+        <v>40.98</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -668,7 +668,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="3">
-        <v>90.88</v>
+        <v>24.87</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -714,7 +714,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="3">
-        <v>193.17</v>
+        <v>109.27</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -783,7 +783,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3">
-        <v>70.98</v>
+        <v>71.08</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -806,7 +806,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="3">
-        <v>121.77</v>
+        <v>101.93</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -829,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="3">
-        <v>262.87</v>
+        <v>250.32</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
@@ -852,7 +852,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="3">
-        <v>147.6</v>
+        <v>84.58</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -898,7 +898,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="3">
-        <v>108.53</v>
+        <v>102.73</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -944,7 +944,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="3">
-        <v>177.88</v>
+        <v>115.17</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -967,7 +967,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="3">
-        <v>218.3</v>
+        <v>74.3</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
@@ -990,7 +990,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="3">
-        <v>273.52</v>
+        <v>104.67</v>
       </c>
       <c r="D22" t="s">
         <v>50</v>
@@ -1013,7 +1013,7 @@
         <v>17</v>
       </c>
       <c r="C23" s="3">
-        <v>174.52</v>
+        <v>96.47</v>
       </c>
       <c r="D23" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Lots of overhauls. Lunch now recognizes Admins (for editing) and has an auto lock for generated times. Scope now works and updates lunch breaks. Configuration has been updated to include Permissions. Tardis now uses new permissions system.
</commit_message>
<xml_diff>
--- a/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
+++ b/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamb\OneDrive\Documents\Scripts\Python\Utilities\time_lord\buildingblocks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{68E56E36-E08B-48C6-B6F4-D6B7FB65219D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-33090" yWindow="3495" windowWidth="28095" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
   <si>
-    <t>Summary report for 12/1/2019 through 12/14/2019</t>
+    <t>Summary report for 12/22/2019 through 1/4/2020</t>
   </si>
   <si>
     <t>payroll_id</t>
@@ -55,10 +61,10 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>12/1/2019</t>
-  </si>
-  <si>
-    <t>12/14/2019</t>
+    <t>12/22/2019</t>
+  </si>
+  <si>
+    <t>1/4/2020</t>
   </si>
   <si>
     <t>Adam</t>
@@ -205,8 +211,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +272,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -312,7 +326,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,9 +358,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,6 +410,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -553,22 +603,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -594,12 +644,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3">
-        <v>28.75</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -617,12 +667,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3">
-        <v>77.34999999999999</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -640,12 +690,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>40.98</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -663,12 +713,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3">
-        <v>24.87</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -686,7 +736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -709,12 +759,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="3">
-        <v>109.27</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -732,12 +782,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3">
-        <v>64.59999999999999</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -755,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -778,12 +828,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3">
-        <v>71.08</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -801,12 +851,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="3">
-        <v>101.93</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -824,12 +874,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="3">
-        <v>250.32</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
@@ -847,12 +897,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="3">
-        <v>84.58</v>
+        <v>0.23</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -870,7 +920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -893,12 +943,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3">
-        <v>102.73</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -916,12 +966,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="3">
-        <v>108.32</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>44</v>
@@ -939,12 +989,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="3">
-        <v>115.17</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -962,12 +1012,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="3">
-        <v>74.3</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
@@ -985,12 +1035,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="3">
-        <v>104.67</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>50</v>
@@ -1008,12 +1058,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="3">
-        <v>96.47</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>52</v>
@@ -1031,7 +1081,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -1054,37 +1104,37 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
I got buttons and gizmos to work in the tree widget, but the problem is that it's not respecting the sub trees, so... I'll have to fix that, but the principle is working.
</commit_message>
<xml_diff>
--- a/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
+++ b/Python/Utilities/time_lord/buildingblocks/Test_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamb\OneDrive\Documents\Scripts\Python\Utilities\time_lord\buildingblocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{68E56E36-E08B-48C6-B6F4-D6B7FB65219D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{48B728A8-E240-47EA-A1E1-F491CFBD0FD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33090" yWindow="3495" windowWidth="28095" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
   <si>
-    <t>Summary report for 12/22/2019 through 1/4/2020</t>
+    <t>Summary report for 12/29/2019 through 1/11/2020</t>
   </si>
   <si>
     <t>payroll_id</t>
@@ -61,10 +61,10 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>12/22/2019</t>
-  </si>
-  <si>
-    <t>1/4/2020</t>
+    <t>12/29/2019</t>
+  </si>
+  <si>
+    <t>1/11/2020</t>
   </si>
   <si>
     <t>Adam</t>
@@ -649,7 +649,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -672,7 +672,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>45.02</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -695,7 +695,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>18.43</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -764,7 +764,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>24.48</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -787,7 +787,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>1.97</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -833,7 +833,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>28.27</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -856,7 +856,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>43.45</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -879,7 +879,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>66.7</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
@@ -902,7 +902,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="3">
-        <v>0.23</v>
+        <v>47.2</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -925,7 +925,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="D17" t="s">
         <v>40</v>
@@ -948,7 +948,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>18.93</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -971,7 +971,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>28.02</v>
       </c>
       <c r="D19" t="s">
         <v>44</v>
@@ -994,7 +994,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>40.42</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -1017,7 +1017,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="3">
-        <v>0.56999999999999995</v>
+        <v>40.17</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
@@ -1040,7 +1040,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>42.73</v>
       </c>
       <c r="D22" t="s">
         <v>50</v>
@@ -1063,7 +1063,7 @@
         <v>17</v>
       </c>
       <c r="C23" s="3">
-        <v>0</v>
+        <v>41.63</v>
       </c>
       <c r="D23" t="s">
         <v>52</v>

</xml_diff>